<commit_message>
Adding markdown and cleaning data
</commit_message>
<xml_diff>
--- a/Austin Wordle Scores.xlsx
+++ b/Austin Wordle Scores.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Wordle Analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59867C23-6948-4835-B059-DEB24080DE63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49DAE416-E7B5-42D0-AC7B-D95477C7138E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="15" windowWidth="29040" windowHeight="15840" xr2:uid="{C3881F8C-4F44-4DCA-B9CC-6B60C92CE002}"/>
   </bookViews>
@@ -392,10 +392,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98338CA3-3593-4AE3-81A9-24997452EF5B}">
-  <dimension ref="A1:B29"/>
+  <dimension ref="A1:B42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -413,55 +413,55 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="B2">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="B3">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="B4">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="B5">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="B6">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="B7">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="B8">
         <v>4</v>
@@ -469,31 +469,31 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="B9">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="B10">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="B11">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="B12">
         <v>4</v>
@@ -501,7 +501,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="B13">
         <v>4</v>
@@ -509,7 +509,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="B14">
         <v>4</v>
@@ -517,15 +517,15 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="B15">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="B16">
         <v>3</v>
@@ -533,52 +533,52 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="B17">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18">
-        <v>334</v>
-      </c>
-      <c r="B18">
-        <v>4</v>
+        <v>335</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19">
-        <v>335</v>
+        <v>336</v>
+      </c>
+      <c r="B19">
+        <v>4</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="B20">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="B21">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="B22">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="B23">
         <v>4</v>
@@ -586,7 +586,7 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="B24">
         <v>4</v>
@@ -594,7 +594,7 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="B25">
         <v>4</v>
@@ -602,34 +602,138 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="B26">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="B27">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="B28">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="B29">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>347</v>
+      </c>
+      <c r="B30">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>348</v>
+      </c>
+      <c r="B31">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>349</v>
+      </c>
+      <c r="B32">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>350</v>
+      </c>
+      <c r="B33">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>351</v>
+      </c>
+      <c r="B34">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>352</v>
+      </c>
+      <c r="B35">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>353</v>
+      </c>
+      <c r="B36">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>354</v>
+      </c>
+      <c r="B37">
         <v>3</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>355</v>
+      </c>
+      <c r="B38">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>356</v>
+      </c>
+      <c r="B39">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>357</v>
+      </c>
+      <c r="B40">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>358</v>
+      </c>
+      <c r="B41">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>359</v>
+      </c>
+      <c r="B42">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
reading in data from SQL database and Excel file
</commit_message>
<xml_diff>
--- a/Austin Wordle Scores.xlsx
+++ b/Austin Wordle Scores.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Wordle Analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49DAE416-E7B5-42D0-AC7B-D95477C7138E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D272212-0596-4FF7-B736-E7078145F09C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="15" windowWidth="29040" windowHeight="15840" xr2:uid="{C3881F8C-4F44-4DCA-B9CC-6B60C92CE002}"/>
   </bookViews>
@@ -35,12 +35,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>WordleDay</t>
   </si>
   <si>
     <t>Score</t>
+  </si>
+  <si>
+    <t>HardMode</t>
   </si>
 </sst>
 </file>
@@ -392,10 +395,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98338CA3-3593-4AE3-81A9-24997452EF5B}">
-  <dimension ref="A1:B42"/>
+  <dimension ref="A1:C42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="E34" sqref="E34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -403,337 +406,463 @@
     <col min="1" max="1" width="10.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>319</v>
       </c>
       <c r="B2">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>320</v>
       </c>
       <c r="B3">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C3" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>321</v>
       </c>
       <c r="B4">
         <v>5</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C4" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>322</v>
       </c>
       <c r="B5">
         <v>2</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C5" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>323</v>
       </c>
       <c r="B6">
         <v>6</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C6" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>324</v>
       </c>
       <c r="B7">
         <v>4</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C7" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>325</v>
       </c>
       <c r="B8">
         <v>4</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C8" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>326</v>
       </c>
       <c r="B9">
         <v>2</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>327</v>
       </c>
       <c r="B10">
         <v>6</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C10" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>328</v>
       </c>
       <c r="B11">
         <v>4</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C11" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>329</v>
       </c>
       <c r="B12">
         <v>4</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C12" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>330</v>
       </c>
       <c r="B13">
         <v>4</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C13" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>331</v>
       </c>
       <c r="B14">
         <v>4</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C14" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>332</v>
       </c>
       <c r="B15">
         <v>3</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C15" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>333</v>
       </c>
       <c r="B16">
         <v>3</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C16" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>334</v>
       </c>
       <c r="B17">
         <v>4</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C17" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>335</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C18" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>336</v>
       </c>
       <c r="B19">
         <v>4</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C19" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>337</v>
       </c>
       <c r="B20">
         <v>5</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C20" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>338</v>
       </c>
       <c r="B21">
         <v>3</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C21" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>339</v>
       </c>
       <c r="B22">
         <v>4</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C22" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>340</v>
       </c>
       <c r="B23">
         <v>4</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C23" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>341</v>
       </c>
       <c r="B24">
         <v>4</v>
       </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C24" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>342</v>
       </c>
       <c r="B25">
         <v>4</v>
       </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C25" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>343</v>
       </c>
       <c r="B26">
         <v>2</v>
       </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C26" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>344</v>
       </c>
       <c r="B27">
         <v>4</v>
       </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C27" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>345</v>
       </c>
       <c r="B28">
         <v>3</v>
       </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C28" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>346</v>
       </c>
       <c r="B29">
         <v>4</v>
       </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C29" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>347</v>
       </c>
       <c r="B30">
         <v>5</v>
       </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C30" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>348</v>
       </c>
       <c r="B31">
         <v>5</v>
       </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C31" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>349</v>
       </c>
       <c r="B32">
         <v>4</v>
       </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C32" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>350</v>
       </c>
       <c r="B33">
         <v>6</v>
       </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C33" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>351</v>
       </c>
       <c r="B34">
         <v>4</v>
       </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C34" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>352</v>
       </c>
       <c r="B35">
         <v>4</v>
       </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C35" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>353</v>
       </c>
       <c r="B36">
         <v>4</v>
       </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C36" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>354</v>
       </c>
       <c r="B37">
         <v>3</v>
       </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C37" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>355</v>
       </c>
       <c r="B38">
         <v>4</v>
       </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C38" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>356</v>
       </c>
       <c r="B39">
         <v>4</v>
       </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C39" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>357</v>
       </c>
       <c r="B40">
         <v>4</v>
       </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C40" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>358</v>
       </c>
       <c r="B41">
         <v>3</v>
       </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C41" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>359</v>
       </c>
       <c r="B42">
         <v>4</v>
+      </c>
+      <c r="C42" t="b">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>